<commit_message>
many new features, bootstrap implemented
</commit_message>
<xml_diff>
--- a/Planification/Libros de Mantención.xlsx
+++ b/Planification/Libros de Mantención.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konko\OneDrive\Documentos\GitHub Repositories\MantencionFishCare\Planification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konko\OneDrive\Documentos\1.- GitHub Repositories\MantencionFishCare\Planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77C5DD6-A3A4-49D2-AFE5-00637950C8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A778C8-B386-4A49-897E-66C1DE6F1020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Digitalizado</t>
   </si>
 </sst>
 </file>
@@ -480,12 +483,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -500,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -516,6 +525,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,9 +822,10 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -824,63 +839,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="8">
         <v>45390</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="G2" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="8">
         <v>45394</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>45404</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>45408</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -891,7 +913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -902,7 +924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -913,7 +935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -924,7 +946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -935,7 +957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -946,7 +968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -957,7 +979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -968,7 +990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -979,7 +1001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>8</v>
       </c>

</xml_diff>